<commit_message>
add coding phase defects
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alest\Downloads\VVSS\01_Tasks\01_Tasks\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate an 3\vvss\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4251EAA3-A8FF-4CBA-9441-B2F288D25D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC5D2D1-8B6C-4386-801F-21A76A90FD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" tabRatio="650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="83">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -210,6 +210,81 @@
   </si>
   <si>
     <t>30 min</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>LinkedTaskList.java/47</t>
+  </si>
+  <si>
+    <t>Task.java/42</t>
+  </si>
+  <si>
+    <t>task is an input parameter which is not checked if its valid or not (null).</t>
+  </si>
+  <si>
+    <t>The condition is (interval &lt; 1) and the message says "interval should me &gt; 1". There is a typo and an error, it should say "interval should be &gt; 0"</t>
+  </si>
+  <si>
+    <t>This condition is all the time true because all of its check components have already been checked before. It introduces confusion.</t>
+  </si>
+  <si>
+    <t>Task.java/107</t>
+  </si>
+  <si>
+    <t>LinkedTaskList.java/98</t>
+  </si>
+  <si>
+    <t>LinkedTaskList.java/15</t>
+  </si>
+  <si>
+    <t>LinkedTaskList.java/39</t>
+  </si>
+  <si>
+    <t>LinkedTaskList.java/60</t>
+  </si>
+  <si>
+    <t>Task.java/25</t>
+  </si>
+  <si>
+    <t>Task.java/134</t>
+  </si>
+  <si>
+    <t>The variable name is tks instead of tasks. At first view, anyone who read the code might get confused because tks does not really have a meaning.</t>
+  </si>
+  <si>
+    <t>cursor variable is not initialized. Initialized it to 0.</t>
+  </si>
+  <si>
+    <t>cursor variable now equals lastCalled which is the index of the removed element. What will happen if we call remove twice? Instead, if it's not the first element, then after removal just decrease the cursor index.</t>
+  </si>
+  <si>
+    <t>this.last is not verified to not be null (empty list) . Added a check for that.</t>
+  </si>
+  <si>
+    <t>Constructor does not have the thorws keyword in the definition even if it can throw an exception. Added it.</t>
+  </si>
+  <si>
+    <t>No need for else; either the function enters the if and then returns or just returns. Removed else.</t>
+  </si>
+  <si>
+    <t>0.5h</t>
+  </si>
+  <si>
+    <t>Silivăstru Oana Maria</t>
   </si>
 </sst>
 </file>
@@ -408,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -439,6 +514,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -481,7 +557,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,40 +869,40 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="59" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.90625" style="6"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -833,73 +911,73 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -913,7 +991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -927,7 +1005,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -942,7 +1020,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -955,7 +1033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="115.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -970,7 +1048,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -985,7 +1063,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1000,7 +1078,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1015,7 +1093,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1024,7 +1102,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1033,7 +1111,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1042,7 +1120,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1051,7 +1129,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1060,7 +1138,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1069,7 +1147,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1078,7 +1156,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1087,7 +1165,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1096,7 +1174,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1126,39 +1204,39 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="22.08984375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="22.140625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1167,57 +1245,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1231,7 +1309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1239,7 +1317,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1248,7 +1326,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1257,7 +1335,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1266,7 +1344,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1275,7 +1353,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1284,7 +1362,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1293,7 +1371,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1302,7 +1380,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1311,7 +1389,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1320,7 +1398,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1329,7 +1407,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1338,7 +1416,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1347,7 +1425,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1356,7 +1434,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1365,7 +1443,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1374,7 +1452,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1383,7 +1461,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1411,40 +1489,40 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1453,60 +1531,66 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I3" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="17">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="D7" s="37">
+        <v>45736</v>
+      </c>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
         <v>5</v>
       </c>
@@ -1517,87 +1601,141 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1606,7 +1744,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1615,7 +1753,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1624,7 +1762,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1633,7 +1771,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1642,7 +1780,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1651,7 +1789,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1660,7 +1798,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1669,7 +1807,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1678,7 +1816,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1687,7 +1825,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1696,7 +1834,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1705,12 +1843,14 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1737,37 +1877,37 @@
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.90625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.90625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="5" max="5" width="23.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1776,47 +1916,47 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1833,7 +1973,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1842,7 +1982,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1852,7 +1992,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1862,7 +2002,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1872,7 +2012,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1882,7 +2022,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1892,7 +2032,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1902,7 +2042,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1912,7 +2052,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1922,7 +2062,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1932,7 +2072,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1942,7 +2082,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1952,7 +2092,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1962,7 +2102,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1972,7 +2112,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1982,7 +2122,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1992,7 +2132,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2002,7 +2142,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2012,7 +2152,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2022,7 +2162,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2032,7 +2172,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2042,15 +2182,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="34" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F35" s="21"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add architectural design phase
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate an 3\vvss\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alest\Downloads\VVSS\01_Tasks\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC5D2D1-8B6C-4386-801F-21A76A90FD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EEE326-B140-40FD-8224-AEC70606D014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" tabRatio="650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="650" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="123">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Tool-based Code Analysis</t>
   </si>
   <si>
-    <t>Effort to perform tool-based code analysis (hours):</t>
-  </si>
-  <si>
     <t>Stoica Alexandra-Maria</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t xml:space="preserve">Nu se mentioneaza ce fel de aplicatie este (mobila, web, desktop etc.)                                                     Nu sunt precizate cerintele hardware/software sau sistemele de operare (Windows/ MacOs/ Linux) necesare pentru a rula aplicatia </t>
   </si>
   <si>
-    <t>30 min</t>
-  </si>
-  <si>
     <t>C06</t>
   </si>
   <si>
@@ -281,17 +275,265 @@
     <t>No need for else; either the function enters the if and then returns or just returns. Removed else.</t>
   </si>
   <si>
-    <t>0.5h</t>
-  </si>
-  <si>
     <t>Silivăstru Oana Maria</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>Arhitectura de tip Model-View-Controller este clar definita.</t>
+  </si>
+  <si>
+    <t>Clasele din subsistem sustin serviciile identificate, conform unei analize initiale.</t>
+  </si>
+  <si>
+    <t>Scopul clasei TasksOperations nu este clar definit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Metodele clasei TasksOperations („incoming” si „calendar”) nu reflecta clar responsabilitatile clasei; se recomanda redenumirea clasei in TasksManager si a metodelor in getIncomingTasks si getCalendarTasks. Clasa ar trebui, de asemenea, sa depinda de TasksService.</t>
+  </si>
+  <si>
+    <t>Relatiile dintre clase sunt corect definite si descriu precis legaturile dintre ele.</t>
+  </si>
+  <si>
+    <t>Clasele entitate si relatiile dintre ele sunt aliniate cu modelele existente si cu cerintele sistemului.</t>
+  </si>
+  <si>
+    <t>Nu este prezentata o strategie clara de gestionare a erorilor.</t>
+  </si>
+  <si>
+    <t>Partitionarea subsistemelor si a pachetelor este logica si coerenta.</t>
+  </si>
+  <si>
+    <t>Toate cerintele au fost verificate si sunt reflectate in diagrama.</t>
+  </si>
+  <si>
+    <t>Stoica Bogdan Andrei</t>
+  </si>
+  <si>
+    <t>Effort to perform tool-based code analysis (hours): 0.5 hours</t>
+  </si>
+  <si>
+    <t>0.5 hours</t>
+  </si>
+  <si>
+    <t>Main.java/27</t>
+  </si>
+  <si>
+    <t>TaskIO.java/26</t>
+  </si>
+  <si>
+    <t>TaskIO.java/79</t>
+  </si>
+  <si>
+    <t>Notificator.java/54</t>
+  </si>
+  <si>
+    <t>NewEditControll.java/79</t>
+  </si>
+  <si>
+    <t>String literals should not be duplicated.</t>
+  </si>
+  <si>
+    <t>Try-with-resources should be used</t>
+  </si>
+  <si>
+    <t>InterruptedException and "ThreadDeath" should not be ignored.</t>
+  </si>
+  <si>
+    <t>"switch" statements should have "default" clauses</t>
+  </si>
+  <si>
+    <t>Unused "private" fields should be removed.</t>
+  </si>
+  <si>
+    <t>Exista un camp privat classLoader care nu era utilizat.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Blocul </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>try</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nu folosea mecanismul </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>try-with-resources</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ceea ce putea duce la scurgeri de resurse.</t>
+    </r>
+  </si>
+  <si>
+    <t>Un anumit string era folosit de mai multe ori in cod, in loc sa fie extras intr-o constanta.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Exceptia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>InterruptedException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> era capturata, dar nu era tratata corespunzator.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Instructiunea </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>switch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nu avea un caz </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ceea ce putea duce la comportamente neprevazute.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Am eliminat campul </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>classLoader</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, deoarece nu era folosit in cod.</t>
+    </r>
+  </si>
+  <si>
+    <t>Am refactorizat codul utilizand try-with-resources pentru a asigura inchiderea automata a resurselor.</t>
+  </si>
+  <si>
+    <t>Am extras string-ul repetitiv intr-o constanta, imbunatatind claritatea si mentenabilitatea codului.</t>
+  </si>
+  <si>
+    <t>Am adaugat Thread.currentThread().interrupt(); pentru a pastra semnalul de intrerupere.</t>
+  </si>
+  <si>
+    <t>Am adaugat un caz default, chiar daca initial nu consideram necesar, pentru a preveni situatii neacoperite.</t>
+  </si>
+  <si>
+    <t>Arhitectura foloseste Model-View-Controller.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,8 +625,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +660,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -483,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -542,6 +801,9 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -557,9 +819,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,23 +1141,23 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A2" zoomScale="83" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -896,7 +1168,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
@@ -911,18 +1183,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -934,13 +1206,13 @@
         <v>21</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
@@ -952,32 +1224,32 @@
         <v>22</v>
       </c>
       <c r="I5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -991,109 +1263,109 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="99" customHeight="1">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="43.5">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17.149999999999999" customHeight="1">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="115.5" customHeight="1">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="72.5">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="87">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    <row r="16" spans="1:10" ht="72.5">
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1102,7 +1374,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1111,7 +1383,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1120,7 +1392,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1129,7 +1401,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1138,7 +1410,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1147,7 +1419,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1156,7 +1428,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1165,7 +1437,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1174,13 +1446,13 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1204,22 +1476,22 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="22.140625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
+    <col min="9" max="9" width="22.1796875" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1230,7 +1502,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
@@ -1245,14 +1517,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1263,10 +1539,14 @@
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1277,25 +1557,33 @@
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="23" t="s">
+        <v>99</v>
+      </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1309,96 +1597,136 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="29">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="101.5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="29">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="41"/>
+      <c r="E18" s="40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="29">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1407,7 +1735,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1416,7 +1744,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1425,7 +1753,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1434,7 +1762,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1443,7 +1771,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1452,7 +1780,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1461,12 +1789,14 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1489,23 +1819,23 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
+    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1516,7 +1846,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
@@ -1531,65 +1861,73 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="17">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="32">
         <v>45736</v>
       </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
         <v>5</v>
@@ -1601,141 +1939,141 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="29">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="58">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="58">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="72.5">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="2" t="s">
+    <row r="16" spans="1:10" ht="29">
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="2" t="s">
+    <row r="17" spans="2:5" ht="43.5">
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
+    <row r="18" spans="2:5" ht="29">
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1744,7 +2082,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1753,7 +2091,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1762,7 +2100,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1771,7 +2109,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1780,7 +2118,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1789,7 +2127,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1798,7 +2136,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1807,7 +2145,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1816,7 +2154,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1825,7 +2163,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1834,7 +2172,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1843,13 +2181,13 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1873,24 +2211,24 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="C1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.81640625" style="6"/>
+    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1901,7 +2239,7 @@
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
@@ -1916,47 +2254,63 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="23" t="s">
+        <v>99</v>
+      </c>
       <c r="E5" s="23"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1973,56 +2327,96 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2032,7 +2426,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2042,7 +2436,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2052,7 +2446,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2062,7 +2456,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2072,7 +2466,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2082,7 +2476,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2092,7 +2486,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2102,7 +2496,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2112,7 +2506,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2122,7 +2516,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2132,7 +2526,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2142,7 +2536,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2152,7 +2546,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2162,7 +2556,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2172,7 +2566,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2182,15 +2576,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+    <row r="32" spans="2:6">
+      <c r="C32" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6">
       <c r="F35" s="21"/>
     </row>
   </sheetData>

</xml_diff>